<commit_message>
added FLEXLAB data from 2/18 with updated SAT upper limit
</commit_message>
<xml_diff>
--- a/data/RTUHPdata/2021-03-12_HP_Filtered.xlsx
+++ b/data/RTUHPdata/2021-03-12_HP_Filtered.xlsx
@@ -90,12 +90,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -110,10 +116,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -399,7 +408,7 @@
   <dimension ref="A1:N182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +438,7 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -447,7 +456,7 @@
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>